<commit_message>
Side by Side Graphs
</commit_message>
<xml_diff>
--- a/Documentation/Stroke.xlsx
+++ b/Documentation/Stroke.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stroke 1.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="157">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -343,6 +343,21 @@
   </si>
   <si>
     <t xml:space="preserve">Not all the features display in x axis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine learning started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaling, Encoding done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strokke 2.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 06 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine learning started.</t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline 1.0</t>
@@ -777,9 +792,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>315720</xdr:colOff>
+      <xdr:colOff>315000</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -793,7 +808,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9545400" cy="4462200"/>
+          <a:ext cx="9544680" cy="4461480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4127,10 +4142,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L985"/>
+  <dimension ref="A1:L986"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4162,10 +4177,10 @@
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4173,41 +4188,43 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="G4" s="4"/>
       <c r="H4" s="2"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
     </row>
@@ -4215,10 +4232,10 @@
       <c r="A7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -4226,19 +4243,19 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="G9" s="4"/>
     </row>
@@ -4246,10 +4263,10 @@
       <c r="A10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -4257,129 +4274,149 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="D14" s="2"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="D18" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="D24" s="2"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="2"/>
       <c r="G25" s="4"/>
     </row>
@@ -4387,17 +4424,18 @@
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="D26" s="2"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="4"/>
       <c r="D27" s="2"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,28 +4465,29 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="D35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4"/>
       <c r="D36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="D39" s="2"/>
     </row>
@@ -4477,6 +4516,7 @@
       <c r="D45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="4"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,7 +4525,7 @@
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7295,6 +7335,9 @@
     </row>
     <row r="985" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D985" s="2"/>
+    </row>
+    <row r="986" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D986" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7345,7 +7388,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
@@ -7354,13 +7397,13 @@
         <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>39</v>
@@ -7369,13 +7412,13 @@
         <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>39</v>
@@ -7384,7 +7427,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="2"/>
@@ -12980,7 +13023,7 @@
   </sheetPr>
   <dimension ref="A1:K987"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -12996,24 +13039,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -13022,10 +13065,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -13034,10 +13077,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="2"/>
@@ -13048,10 +13091,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -13060,10 +13103,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -13072,7 +13115,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2"/>
       <c r="F7" s="4"/>
@@ -13082,50 +13125,50 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
       <c r="B9" s="16" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14"/>
       <c r="B10" s="16" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14"/>
       <c r="B11" s="16" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14"/>
       <c r="B12" s="16" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -13133,7 +13176,7 @@
       <c r="A13" s="14"/>
       <c r="B13" s="16"/>
       <c r="C13" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -13141,17 +13184,17 @@
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14"/>
       <c r="B15" s="16" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -13159,17 +13202,17 @@
       <c r="A16" s="14"/>
       <c r="B16" s="16"/>
       <c r="C16" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14"/>
       <c r="B17" s="16" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -16177,24 +16220,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -16209,10 +16252,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="2"/>
@@ -16223,10 +16266,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -16235,10 +16278,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -16247,10 +16290,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -16259,10 +16302,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F8" s="4"/>
     </row>

</xml_diff>